<commit_message>
Added styling. Added two data viz's to index. Cleaned data wrangling code.
</commit_message>
<xml_diff>
--- a/cleaned data/Cities.xlsx
+++ b/cleaned data/Cities.xlsx
@@ -14,18 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="145">
   <si>
     <t>Home Sales</t>
   </si>
   <si>
     <t>Median Sales Price</t>
-  </si>
-  <si>
-    <t>Thousands Of Residents</t>
-  </si>
-  <si>
-    <t>Per Capita Personal Income</t>
   </si>
   <si>
     <t>Sales Per Thousand Residents</t>
@@ -812,15 +806,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -834,16 +828,10 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -852,21 +840,15 @@
         <v>210000</v>
       </c>
       <c r="D2">
-        <v>179.308</v>
+        <v>0.03346197604122515</v>
       </c>
       <c r="E2">
-        <v>55556</v>
-      </c>
-      <c r="F2">
-        <v>0.03346197604122515</v>
-      </c>
-      <c r="G2">
         <v>3.779969760241918</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>25</v>
@@ -875,21 +857,15 @@
         <v>164900</v>
       </c>
       <c r="D3">
-        <v>697.627</v>
+        <v>0.03583576897109774</v>
       </c>
       <c r="E3">
-        <v>58735</v>
-      </c>
-      <c r="F3">
-        <v>0.03583576897109774</v>
-      </c>
-      <c r="G3">
         <v>2.807525325615051</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>49</v>
@@ -898,21 +874,15 @@
         <v>333500</v>
       </c>
       <c r="D4">
-        <v>919.543</v>
+        <v>0.05328733947188984</v>
       </c>
       <c r="E4">
-        <v>52263</v>
-      </c>
-      <c r="F4">
-        <v>0.05328733947188984</v>
-      </c>
-      <c r="G4">
         <v>6.381187455752635</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -921,21 +891,15 @@
         <v>152000</v>
       </c>
       <c r="D5">
-        <v>271.171</v>
+        <v>0.02581396978290451</v>
       </c>
       <c r="E5">
-        <v>56248</v>
-      </c>
-      <c r="F5">
-        <v>0.02581396978290451</v>
-      </c>
-      <c r="G5">
         <v>2.702318304650832</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -944,21 +908,15 @@
         <v>309900</v>
       </c>
       <c r="D6">
-        <v>126.282</v>
+        <v>0.007918784941638555</v>
       </c>
       <c r="E6">
-        <v>49320</v>
-      </c>
-      <c r="F6">
-        <v>0.007918784941638555</v>
-      </c>
-      <c r="G6">
         <v>6.28345498783455</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -967,21 +925,15 @@
         <v>279500</v>
       </c>
       <c r="D7">
-        <v>400.47</v>
+        <v>0.02497065947511674</v>
       </c>
       <c r="E7">
-        <v>67085</v>
-      </c>
-      <c r="F7">
-        <v>0.02497065947511674</v>
-      </c>
-      <c r="G7">
         <v>4.166356115376016</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>26</v>
@@ -990,9 +942,9 @@
         <v>194950</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -1001,21 +953,15 @@
         <v>267250</v>
       </c>
       <c r="D9">
-        <v>244.845</v>
+        <v>0.0163368661806449</v>
       </c>
       <c r="E9">
-        <v>58312</v>
-      </c>
-      <c r="F9">
-        <v>0.0163368661806449</v>
-      </c>
-      <c r="G9">
         <v>4.583104678282344</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1024,21 +970,15 @@
         <v>509000</v>
       </c>
       <c r="D10">
-        <v>476.072</v>
+        <v>0.01890470349022837</v>
       </c>
       <c r="E10">
-        <v>54827</v>
-      </c>
-      <c r="F10">
-        <v>0.01890470349022837</v>
-      </c>
-      <c r="G10">
         <v>9.283747058930819</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1047,21 +987,15 @@
         <v>347450</v>
       </c>
       <c r="D11">
-        <v>916.1079999999999</v>
+        <v>0.01091574355861973</v>
       </c>
       <c r="E11">
-        <v>45961</v>
-      </c>
-      <c r="F11">
-        <v>0.01091574355861973</v>
-      </c>
-      <c r="G11">
         <v>7.559670155131524</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -1070,21 +1004,15 @@
         <v>419990</v>
       </c>
       <c r="D12">
-        <v>230.677</v>
+        <v>0.0130051977440317</v>
       </c>
       <c r="E12">
-        <v>58137</v>
-      </c>
-      <c r="F12">
-        <v>0.0130051977440317</v>
-      </c>
-      <c r="G12">
         <v>7.224142972633607</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1093,21 +1021,15 @@
         <v>339500</v>
       </c>
       <c r="D13">
-        <v>190.208</v>
+        <v>0.03154441453566622</v>
       </c>
       <c r="E13">
-        <v>59698</v>
-      </c>
-      <c r="F13">
-        <v>0.03154441453566622</v>
-      </c>
-      <c r="G13">
         <v>5.686957687024691</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>12</v>
@@ -1116,21 +1038,15 @@
         <v>281950</v>
       </c>
       <c r="D14">
-        <v>134.846</v>
+        <v>0.08899040386811621</v>
       </c>
       <c r="E14">
-        <v>64134</v>
-      </c>
-      <c r="F14">
-        <v>0.08899040386811621</v>
-      </c>
-      <c r="G14">
         <v>4.396264072099043</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>11</v>
@@ -1139,15 +1055,12 @@
         <v>269900</v>
       </c>
       <c r="D15">
-        <v>171.141</v>
-      </c>
-      <c r="F15">
         <v>0.06427448711880847</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>11</v>
@@ -1156,9 +1069,9 @@
         <v>269900</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>11</v>
@@ -1167,21 +1080,15 @@
         <v>299000</v>
       </c>
       <c r="D17">
-        <v>161.227</v>
+        <v>0.06822678583611926</v>
       </c>
       <c r="E17">
-        <v>51899</v>
-      </c>
-      <c r="F17">
-        <v>0.06822678583611926</v>
-      </c>
-      <c r="G17">
         <v>5.761190003660957</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -1190,21 +1097,15 @@
         <v>971750</v>
       </c>
       <c r="D18">
-        <v>327.468</v>
+        <v>0.01221493397828185</v>
       </c>
       <c r="E18">
-        <v>89593</v>
-      </c>
-      <c r="F18">
-        <v>0.01221493397828185</v>
-      </c>
-      <c r="G18">
         <v>10.84627147210161</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>11</v>
@@ -1213,21 +1114,15 @@
         <v>249999</v>
       </c>
       <c r="D19">
-        <v>176.353</v>
+        <v>0.06237489580557178</v>
       </c>
       <c r="E19">
-        <v>48118</v>
-      </c>
-      <c r="F19">
-        <v>0.06237489580557178</v>
-      </c>
-      <c r="G19">
         <v>5.19554013051249</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>12</v>
@@ -1236,21 +1131,15 @@
         <v>275000</v>
       </c>
       <c r="D20">
-        <v>79.601</v>
+        <v>0.150751874976445</v>
       </c>
       <c r="E20">
-        <v>70175</v>
-      </c>
-      <c r="F20">
-        <v>0.150751874976445</v>
-      </c>
-      <c r="G20">
         <v>3.918774492340577</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -1259,21 +1148,15 @@
         <v>149900</v>
       </c>
       <c r="D21">
-        <v>251.914</v>
+        <v>0.01984804337988361</v>
       </c>
       <c r="E21">
-        <v>51638</v>
-      </c>
-      <c r="F21">
-        <v>0.01984804337988361</v>
-      </c>
-      <c r="G21">
         <v>2.902900964406057</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -1282,21 +1165,15 @@
         <v>460000</v>
       </c>
       <c r="D22">
-        <v>223.825</v>
+        <v>0.09382329945269742</v>
       </c>
       <c r="E22">
-        <v>77070</v>
-      </c>
-      <c r="F22">
-        <v>0.09382329945269742</v>
-      </c>
-      <c r="G22">
         <v>5.968599974049566</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>6</v>
@@ -1305,21 +1182,15 @@
         <v>354500</v>
       </c>
       <c r="D23">
-        <v>207.303</v>
+        <v>0.02894314119911434</v>
       </c>
       <c r="E23">
-        <v>54694</v>
-      </c>
-      <c r="F23">
-        <v>0.02894314119911434</v>
-      </c>
-      <c r="G23">
         <v>6.48151533989103</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>14</v>
@@ -1328,21 +1199,15 @@
         <v>307450</v>
       </c>
       <c r="D24">
-        <v>214.63</v>
+        <v>0.06522853282392956</v>
       </c>
       <c r="E24">
-        <v>53583</v>
-      </c>
-      <c r="F24">
-        <v>0.06522853282392956</v>
-      </c>
-      <c r="G24">
         <v>5.737827295970737</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1351,21 +1216,15 @@
         <v>220000</v>
       </c>
       <c r="D25">
-        <v>847.686</v>
+        <v>0.001179682099267889</v>
       </c>
       <c r="E25">
-        <v>53286</v>
-      </c>
-      <c r="F25">
-        <v>0.001179682099267889</v>
-      </c>
-      <c r="G25">
         <v>4.128664189468153</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>8</v>
@@ -1374,21 +1233,15 @@
         <v>217500</v>
       </c>
       <c r="D26">
-        <v>83.54000000000001</v>
+        <v>0.09576250897773521</v>
       </c>
       <c r="E26">
-        <v>61136</v>
-      </c>
-      <c r="F26">
-        <v>0.09576250897773521</v>
-      </c>
-      <c r="G26">
         <v>3.557641978539649</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>87</v>
@@ -1397,21 +1250,15 @@
         <v>270000</v>
       </c>
       <c r="D27">
-        <v>2161.511</v>
+        <v>0.0402496216766882</v>
       </c>
       <c r="E27">
-        <v>59867</v>
-      </c>
-      <c r="F27">
-        <v>0.0402496216766882</v>
-      </c>
-      <c r="G27">
         <v>4.509997160372158</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>4</v>
@@ -1420,21 +1267,15 @@
         <v>402000</v>
       </c>
       <c r="D28">
-        <v>97.63</v>
+        <v>0.04097101300829663</v>
       </c>
       <c r="E28">
-        <v>54174</v>
-      </c>
-      <c r="F28">
-        <v>0.04097101300829663</v>
-      </c>
-      <c r="G28">
         <v>7.420533835419205</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -1443,21 +1284,15 @@
         <v>45000</v>
       </c>
       <c r="D29">
-        <v>72.337</v>
+        <v>0.04147255208261332</v>
       </c>
       <c r="E29">
-        <v>49265</v>
-      </c>
-      <c r="F29">
-        <v>0.04147255208261332</v>
-      </c>
-      <c r="G29">
         <v>0.9134273825230894</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>61</v>
@@ -1466,15 +1301,12 @@
         <v>199900</v>
       </c>
       <c r="D30">
-        <v>812.595</v>
-      </c>
-      <c r="F30">
         <v>0.07506814587832807</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>6</v>
@@ -1483,21 +1315,15 @@
         <v>301707</v>
       </c>
       <c r="D31">
-        <v>157.425</v>
+        <v>0.03811338732729871</v>
       </c>
       <c r="E31">
-        <v>46533</v>
-      </c>
-      <c r="F31">
-        <v>0.03811338732729871</v>
-      </c>
-      <c r="G31">
         <v>6.483721230094772</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>4</v>
@@ -1506,21 +1332,15 @@
         <v>122200</v>
       </c>
       <c r="D32">
-        <v>101.483</v>
+        <v>0.03941546860065232</v>
       </c>
       <c r="E32">
-        <v>56548</v>
-      </c>
-      <c r="F32">
-        <v>0.03941546860065232</v>
-      </c>
-      <c r="G32">
         <v>2.160995968027163</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -1529,21 +1349,15 @@
         <v>290000</v>
       </c>
       <c r="D33">
-        <v>186.946</v>
+        <v>0.02139655301530924</v>
       </c>
       <c r="E33">
-        <v>50432</v>
-      </c>
-      <c r="F33">
-        <v>0.02139655301530924</v>
-      </c>
-      <c r="G33">
         <v>5.750317258883249</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -1552,21 +1366,15 @@
         <v>225000</v>
       </c>
       <c r="D34">
-        <v>98.67700000000001</v>
+        <v>0.05067036898162692</v>
       </c>
       <c r="E34">
-        <v>56782</v>
-      </c>
-      <c r="F34">
-        <v>0.05067036898162692</v>
-      </c>
-      <c r="G34">
         <v>3.962523334859639</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>4</v>
@@ -1575,21 +1383,15 @@
         <v>145950</v>
       </c>
       <c r="D35">
-        <v>81.426</v>
+        <v>0.04912435831306954</v>
       </c>
       <c r="E35">
-        <v>52360</v>
-      </c>
-      <c r="F35">
-        <v>0.04912435831306954</v>
-      </c>
-      <c r="G35">
         <v>2.787433155080214</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>20</v>
@@ -1598,21 +1400,15 @@
         <v>154900</v>
       </c>
       <c r="D36">
-        <v>267.689</v>
+        <v>0.07471356686303882</v>
       </c>
       <c r="E36">
-        <v>52747</v>
-      </c>
-      <c r="F36">
-        <v>0.07471356686303882</v>
-      </c>
-      <c r="G36">
         <v>2.936659904828711</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>10</v>
@@ -1621,21 +1417,15 @@
         <v>476950</v>
       </c>
       <c r="D37">
-        <v>382.353</v>
+        <v>0.02615384213017813</v>
       </c>
       <c r="E37">
-        <v>55146</v>
-      </c>
-      <c r="F37">
-        <v>0.02615384213017813</v>
-      </c>
-      <c r="G37">
         <v>8.648859391433648</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -1644,21 +1434,15 @@
         <v>292450</v>
       </c>
       <c r="D38">
-        <v>120.418</v>
+        <v>0.01660881263598465</v>
       </c>
       <c r="E38">
-        <v>41735</v>
-      </c>
-      <c r="F38">
-        <v>0.01660881263598465</v>
-      </c>
-      <c r="G38">
         <v>7.007308014855637</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -1667,21 +1451,15 @@
         <v>199950</v>
       </c>
       <c r="D39">
-        <v>529.318</v>
+        <v>0.07179049267170208</v>
       </c>
       <c r="E39">
-        <v>45542</v>
-      </c>
-      <c r="F39">
-        <v>0.07179049267170208</v>
-      </c>
-      <c r="G39">
         <v>4.390452768872689</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40">
         <v>6</v>
@@ -1690,21 +1468,15 @@
         <v>599950</v>
       </c>
       <c r="D40">
-        <v>144.06</v>
+        <v>0.04164931278633902</v>
       </c>
       <c r="E40">
-        <v>56914</v>
-      </c>
-      <c r="F40">
-        <v>0.04164931278633902</v>
-      </c>
-      <c r="G40">
         <v>10.54134307903152</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B41">
         <v>11</v>
@@ -1713,21 +1485,15 @@
         <v>130000</v>
       </c>
       <c r="D41">
-        <v>401.983</v>
+        <v>0.02736434127811375</v>
       </c>
       <c r="E41">
-        <v>49399</v>
-      </c>
-      <c r="F41">
-        <v>0.02736434127811375</v>
-      </c>
-      <c r="G41">
         <v>2.631632219275694</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B42">
         <v>8</v>
@@ -1736,21 +1502,15 @@
         <v>160000</v>
       </c>
       <c r="D42">
-        <v>199.119</v>
+        <v>0.04017697959511649</v>
       </c>
       <c r="E42">
-        <v>50386</v>
-      </c>
-      <c r="F42">
-        <v>0.04017697959511649</v>
-      </c>
-      <c r="G42">
         <v>3.175485253840352</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B43">
         <v>15</v>
@@ -1759,21 +1519,15 @@
         <v>350000</v>
       </c>
       <c r="D43">
-        <v>1015.19</v>
+        <v>0.0147755592549178</v>
       </c>
       <c r="E43">
-        <v>51422</v>
-      </c>
-      <c r="F43">
-        <v>0.0147755592549178</v>
-      </c>
-      <c r="G43">
         <v>6.806425265450585</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -1782,21 +1536,15 @@
         <v>107700</v>
       </c>
       <c r="D44">
-        <v>103.088</v>
+        <v>0.01940090020176936</v>
       </c>
       <c r="E44">
-        <v>42558</v>
-      </c>
-      <c r="F44">
-        <v>0.01940090020176936</v>
-      </c>
-      <c r="G44">
         <v>2.530664034964049</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B45">
         <v>14</v>
@@ -1805,21 +1553,15 @@
         <v>297450</v>
       </c>
       <c r="D45">
-        <v>348.282</v>
+        <v>0.04019731137411638</v>
       </c>
       <c r="E45">
-        <v>50623</v>
-      </c>
-      <c r="F45">
-        <v>0.04019731137411638</v>
-      </c>
-      <c r="G45">
         <v>5.875787685439425</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B46">
         <v>21</v>
@@ -1828,21 +1570,15 @@
         <v>390515</v>
       </c>
       <c r="D46">
-        <v>212.692</v>
+        <v>0.09873432004964926</v>
       </c>
       <c r="E46">
-        <v>53920</v>
-      </c>
-      <c r="F46">
-        <v>0.09873432004964926</v>
-      </c>
-      <c r="G46">
         <v>7.242488872403561</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -1851,21 +1587,15 @@
         <v>467900</v>
       </c>
       <c r="D47">
-        <v>117.286</v>
+        <v>0.008526166805927391</v>
       </c>
       <c r="E47">
-        <v>49881</v>
-      </c>
-      <c r="F47">
-        <v>0.008526166805927391</v>
-      </c>
-      <c r="G47">
         <v>9.380325173913915</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <v>11</v>
@@ -1874,21 +1604,15 @@
         <v>365000</v>
       </c>
       <c r="D48">
-        <v>350.176</v>
+        <v>0.03141277529013982</v>
       </c>
       <c r="E48">
-        <v>56553</v>
-      </c>
-      <c r="F48">
-        <v>0.03141277529013982</v>
-      </c>
-      <c r="G48">
         <v>6.45412268137853</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B49">
         <v>11</v>
@@ -1897,21 +1621,15 @@
         <v>200000</v>
       </c>
       <c r="D49">
-        <v>173.542</v>
+        <v>0.06338523239331113</v>
       </c>
       <c r="E49">
-        <v>53200</v>
-      </c>
-      <c r="F49">
-        <v>0.06338523239331113</v>
-      </c>
-      <c r="G49">
         <v>3.759398496240602</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -1920,21 +1638,15 @@
         <v>230000</v>
       </c>
       <c r="D50">
-        <v>136.555</v>
+        <v>0.01464611328768628</v>
       </c>
       <c r="E50">
-        <v>47217</v>
-      </c>
-      <c r="F50">
-        <v>0.01464611328768628</v>
-      </c>
-      <c r="G50">
         <v>4.871126924624606</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -1943,21 +1655,15 @@
         <v>229000</v>
       </c>
       <c r="D51">
-        <v>173.359</v>
+        <v>0.01730512981731551</v>
       </c>
       <c r="E51">
-        <v>44538</v>
-      </c>
-      <c r="F51">
-        <v>0.01730512981731551</v>
-      </c>
-      <c r="G51">
         <v>5.141676770398312</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B52">
         <v>6</v>
@@ -1966,21 +1672,15 @@
         <v>258750</v>
       </c>
       <c r="D52">
-        <v>86.378</v>
+        <v>0.06946213156127717</v>
       </c>
       <c r="E52">
-        <v>41012</v>
-      </c>
-      <c r="F52">
-        <v>0.06946213156127717</v>
-      </c>
-      <c r="G52">
         <v>6.309129035404272</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B53">
         <v>2</v>
@@ -1989,21 +1689,15 @@
         <v>548650</v>
       </c>
       <c r="D53">
-        <v>514.465</v>
+        <v>0.00388753365146317</v>
       </c>
       <c r="E53">
-        <v>57815</v>
-      </c>
-      <c r="F53">
-        <v>0.00388753365146317</v>
-      </c>
-      <c r="G53">
         <v>9.489751794516994</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -2012,21 +1706,15 @@
         <v>465000</v>
       </c>
       <c r="D54">
-        <v>104.777</v>
+        <v>0.009544079330387393</v>
       </c>
       <c r="E54">
-        <v>51377</v>
-      </c>
-      <c r="F54">
-        <v>0.009544079330387393</v>
-      </c>
-      <c r="G54">
         <v>9.050742550168364</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B55">
         <v>11</v>
@@ -2035,21 +1723,15 @@
         <v>129900</v>
       </c>
       <c r="D55">
-        <v>160.066</v>
+        <v>0.06872165231841865</v>
       </c>
       <c r="E55">
-        <v>47503</v>
-      </c>
-      <c r="F55">
-        <v>0.06872165231841865</v>
-      </c>
-      <c r="G55">
         <v>2.734564132791613</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B56">
         <v>5</v>
@@ -2058,21 +1740,15 @@
         <v>229614</v>
       </c>
       <c r="D56">
-        <v>583.197</v>
+        <v>0.008573432305035862</v>
       </c>
       <c r="E56">
-        <v>51982</v>
-      </c>
-      <c r="F56">
-        <v>0.008573432305035862</v>
-      </c>
-      <c r="G56">
         <v>4.417182870993805</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -2081,21 +1757,15 @@
         <v>180000</v>
       </c>
       <c r="D57">
-        <v>181.579</v>
+        <v>0.01101448956101752</v>
       </c>
       <c r="E57">
-        <v>48718</v>
-      </c>
-      <c r="F57">
-        <v>0.01101448956101752</v>
-      </c>
-      <c r="G57">
         <v>3.694732952912681</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B58">
         <v>94</v>
@@ -2104,21 +1774,15 @@
         <v>299450</v>
       </c>
       <c r="D58">
-        <v>1675.668</v>
+        <v>0.05609703115414271</v>
       </c>
       <c r="E58">
-        <v>59271</v>
-      </c>
-      <c r="F58">
-        <v>0.05609703115414271</v>
-      </c>
-      <c r="G58">
         <v>5.052217779352466</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B59">
         <v>19</v>
@@ -2127,21 +1791,15 @@
         <v>195000</v>
       </c>
       <c r="D59">
-        <v>207.298</v>
+        <v>0.09165549112871325</v>
       </c>
       <c r="E59">
-        <v>50869</v>
-      </c>
-      <c r="F59">
-        <v>0.09165549112871325</v>
-      </c>
-      <c r="G59">
         <v>3.833375926399182</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B60">
         <v>9</v>
@@ -2150,21 +1808,15 @@
         <v>220000</v>
       </c>
       <c r="D60">
-        <v>135.512</v>
+        <v>0.06641478245469036</v>
       </c>
       <c r="E60">
-        <v>44554</v>
-      </c>
-      <c r="F60">
-        <v>0.06641478245469036</v>
-      </c>
-      <c r="G60">
         <v>4.937828253355478</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B61">
         <v>7</v>
@@ -2173,21 +1825,15 @@
         <v>213500</v>
       </c>
       <c r="D61">
-        <v>184.086</v>
+        <v>0.03802570537683474</v>
       </c>
       <c r="E61">
-        <v>44292</v>
-      </c>
-      <c r="F61">
-        <v>0.03802570537683474</v>
-      </c>
-      <c r="G61">
         <v>4.820283572654204</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -2196,21 +1842,15 @@
         <v>39000</v>
       </c>
       <c r="D62">
-        <v>106.074</v>
+        <v>0.009427380885042518</v>
       </c>
       <c r="E62">
-        <v>53165</v>
-      </c>
-      <c r="F62">
-        <v>0.009427380885042518</v>
-      </c>
-      <c r="G62">
         <v>0.7335653155271326</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B63">
         <v>4</v>
@@ -2219,21 +1859,15 @@
         <v>519450</v>
       </c>
       <c r="D63">
-        <v>182.319</v>
+        <v>0.0219395674614275</v>
       </c>
       <c r="E63">
-        <v>60557</v>
-      </c>
-      <c r="F63">
-        <v>0.0219395674614275</v>
-      </c>
-      <c r="G63">
         <v>8.57786878478128</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B64">
         <v>65</v>
@@ -2242,21 +1876,15 @@
         <v>364900</v>
       </c>
       <c r="D64">
-        <v>907.968</v>
+        <v>0.07158842602382463</v>
       </c>
       <c r="E64">
-        <v>55752</v>
-      </c>
-      <c r="F64">
-        <v>0.07158842602382463</v>
-      </c>
-      <c r="G64">
         <v>6.545056679581002</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B65">
         <v>5</v>
@@ -2265,21 +1893,15 @@
         <v>129900</v>
       </c>
       <c r="D65">
-        <v>83.574</v>
+        <v>0.0598272189915524</v>
       </c>
       <c r="E65">
-        <v>47031</v>
-      </c>
-      <c r="F65">
-        <v>0.0598272189915524</v>
-      </c>
-      <c r="G65">
         <v>2.762008037252025</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:5">
       <c r="A66" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B66">
         <v>11</v>
@@ -2288,21 +1910,15 @@
         <v>240500</v>
       </c>
       <c r="D66">
-        <v>481.125</v>
+        <v>0.02286308131982333</v>
       </c>
       <c r="E66">
-        <v>52241</v>
-      </c>
-      <c r="F66">
-        <v>0.02286308131982333</v>
-      </c>
-      <c r="G66">
         <v>4.603663788978006</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B67">
         <v>7</v>
@@ -2311,21 +1927,15 @@
         <v>275900</v>
       </c>
       <c r="D67">
-        <v>556.629</v>
+        <v>0.01257570123008323</v>
       </c>
       <c r="E67">
-        <v>61547</v>
-      </c>
-      <c r="F67">
-        <v>0.01257570123008323</v>
-      </c>
-      <c r="G67">
         <v>4.48275301801875</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2334,21 +1944,15 @@
         <v>165000</v>
       </c>
       <c r="D68">
-        <v>267.78</v>
+        <v>0.003734408843080141</v>
       </c>
       <c r="E68">
-        <v>40850</v>
-      </c>
-      <c r="F68">
-        <v>0.003734408843080141</v>
-      </c>
-      <c r="G68">
         <v>4.039167686658507</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B69">
         <v>7</v>
@@ -2357,21 +1961,15 @@
         <v>369900</v>
       </c>
       <c r="D69">
-        <v>119.964</v>
+        <v>0.0583508385849088</v>
       </c>
       <c r="E69">
-        <v>51703</v>
-      </c>
-      <c r="F69">
-        <v>0.0583508385849088</v>
-      </c>
-      <c r="G69">
         <v>7.154323733632478</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:5">
       <c r="A70" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B70">
         <v>13</v>
@@ -2380,21 +1978,15 @@
         <v>155000</v>
       </c>
       <c r="D70">
-        <v>128.523</v>
+        <v>0.1011492106471215</v>
       </c>
       <c r="E70">
-        <v>47807</v>
-      </c>
-      <c r="F70">
-        <v>0.1011492106471215</v>
-      </c>
-      <c r="G70">
         <v>3.24220302466166</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B71">
         <v>5</v>
@@ -2403,21 +1995,15 @@
         <v>214900</v>
       </c>
       <c r="D71">
-        <v>144.011</v>
+        <v>0.03471957003284471</v>
       </c>
       <c r="E71">
-        <v>55803</v>
-      </c>
-      <c r="F71">
-        <v>0.03471957003284471</v>
-      </c>
-      <c r="G71">
         <v>3.851047434725732</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:5">
       <c r="A72" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B72">
         <v>30</v>
@@ -2426,21 +2012,15 @@
         <v>268500</v>
       </c>
       <c r="D72">
-        <v>342.448</v>
+        <v>0.08760454141942718</v>
       </c>
       <c r="E72">
-        <v>56887</v>
-      </c>
-      <c r="F72">
-        <v>0.08760454141942718</v>
-      </c>
-      <c r="G72">
         <v>4.719883277374444</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:5">
       <c r="A73" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B73">
         <v>2</v>
@@ -2449,21 +2029,15 @@
         <v>248250</v>
       </c>
       <c r="D73">
-        <v>291.219</v>
+        <v>0.006867683770633098</v>
       </c>
       <c r="E73">
-        <v>48868</v>
-      </c>
-      <c r="F73">
-        <v>0.006867683770633098</v>
-      </c>
-      <c r="G73">
         <v>5.080011459441762</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:5">
       <c r="A74" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B74">
         <v>4</v>
@@ -2472,21 +2046,15 @@
         <v>272450</v>
       </c>
       <c r="D74">
-        <v>111.956</v>
+        <v>0.03572832184072314</v>
       </c>
       <c r="E74">
-        <v>54550</v>
-      </c>
-      <c r="F74">
-        <v>0.03572832184072314</v>
-      </c>
-      <c r="G74">
         <v>4.994500458295142</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:5">
       <c r="A75" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B75">
         <v>24</v>
@@ -2495,21 +2063,15 @@
         <v>262750</v>
       </c>
       <c r="D75">
-        <v>328.283</v>
+        <v>0.07310765406676556</v>
       </c>
       <c r="E75">
-        <v>51045</v>
-      </c>
-      <c r="F75">
-        <v>0.07310765406676556</v>
-      </c>
-      <c r="G75">
         <v>5.147418944068959</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B76">
         <v>11</v>
@@ -2518,21 +2080,15 @@
         <v>299900</v>
       </c>
       <c r="D76">
-        <v>263.613</v>
+        <v>0.04172783588062804</v>
       </c>
       <c r="E76">
-        <v>47374</v>
-      </c>
-      <c r="F76">
-        <v>0.04172783588062804</v>
-      </c>
-      <c r="G76">
         <v>6.330476632752142</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:5">
       <c r="A77" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B77">
         <v>2</v>
@@ -2541,21 +2097,15 @@
         <v>507750</v>
       </c>
       <c r="D77">
-        <v>160.256</v>
+        <v>0.01248003194888179</v>
       </c>
       <c r="E77">
-        <v>45757</v>
-      </c>
-      <c r="F77">
-        <v>0.01248003194888179</v>
-      </c>
-      <c r="G77">
         <v>11.09666280569093</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:5">
       <c r="A78" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -2564,21 +2114,15 @@
         <v>379900</v>
       </c>
       <c r="D78">
-        <v>687.077</v>
+        <v>0.02328705516266736</v>
       </c>
       <c r="E78">
-        <v>69116</v>
-      </c>
-      <c r="F78">
-        <v>0.02328705516266736</v>
-      </c>
-      <c r="G78">
         <v>5.496556513687135</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:5">
       <c r="A79" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B79">
         <v>7</v>
@@ -2587,21 +2131,15 @@
         <v>149900</v>
       </c>
       <c r="D79">
-        <v>125.319</v>
+        <v>0.05585745178304966</v>
       </c>
       <c r="E79">
-        <v>46366</v>
-      </c>
-      <c r="F79">
-        <v>0.05585745178304966</v>
-      </c>
-      <c r="G79">
         <v>3.232972436699305</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:5">
       <c r="A80" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B80">
         <v>3</v>
@@ -2610,21 +2148,15 @@
         <v>450000</v>
       </c>
       <c r="D80">
-        <v>221.644</v>
+        <v>0.01353521863889841</v>
       </c>
       <c r="E80">
-        <v>56842</v>
-      </c>
-      <c r="F80">
-        <v>0.01353521863889841</v>
-      </c>
-      <c r="G80">
         <v>7.916681327187643</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:5">
       <c r="A81" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B81">
         <v>4</v>
@@ -2633,21 +2165,15 @@
         <v>427995</v>
       </c>
       <c r="D81">
-        <v>290.014</v>
+        <v>0.01379243760646038</v>
       </c>
       <c r="E81">
-        <v>46580</v>
-      </c>
-      <c r="F81">
-        <v>0.01379243760646038</v>
-      </c>
-      <c r="G81">
         <v>9.188385573207386</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:5">
       <c r="A82" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -2656,21 +2182,15 @@
         <v>385000</v>
       </c>
       <c r="D82">
-        <v>177.216</v>
+        <v>0.02257132538822679</v>
       </c>
       <c r="E82">
-        <v>125455</v>
-      </c>
-      <c r="F82">
-        <v>0.02257132538822679</v>
-      </c>
-      <c r="G82">
         <v>3.068829460762823</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:5">
       <c r="A83" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B83">
         <v>11</v>
@@ -2679,21 +2199,15 @@
         <v>649000</v>
       </c>
       <c r="D83">
-        <v>121.041</v>
+        <v>0.09087829743640585</v>
       </c>
       <c r="E83">
-        <v>61881</v>
-      </c>
-      <c r="F83">
-        <v>0.09087829743640585</v>
-      </c>
-      <c r="G83">
         <v>10.48787188313053</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:5">
       <c r="A84" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B84">
         <v>22</v>
@@ -2702,21 +2216,15 @@
         <v>219900</v>
       </c>
       <c r="D84">
-        <v>426.533</v>
+        <v>0.05157865862664788</v>
       </c>
       <c r="E84">
-        <v>46402</v>
-      </c>
-      <c r="F84">
-        <v>0.05157865862664788</v>
-      </c>
-      <c r="G84">
         <v>4.739019869833196</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:5">
       <c r="A85" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -2725,21 +2233,15 @@
         <v>517450</v>
       </c>
       <c r="D85">
-        <v>551.275</v>
+        <v>0.003627953380799057</v>
       </c>
       <c r="E85">
-        <v>52356</v>
-      </c>
-      <c r="F85">
-        <v>0.003627953380799057</v>
-      </c>
-      <c r="G85">
         <v>9.883298953319581</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:5">
       <c r="A86" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -2748,21 +2250,15 @@
         <v>134900</v>
       </c>
       <c r="D86">
-        <v>202.869</v>
+        <v>0.004929289344355224</v>
       </c>
       <c r="E86">
-        <v>46859</v>
-      </c>
-      <c r="F86">
-        <v>0.004929289344355224</v>
-      </c>
-      <c r="G86">
         <v>2.878849313899144</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:5">
       <c r="A87" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B87">
         <v>6</v>
@@ -2771,21 +2267,15 @@
         <v>362450</v>
       </c>
       <c r="D87">
-        <v>155.609</v>
+        <v>0.03855818108207108</v>
       </c>
       <c r="E87">
-        <v>53509</v>
-      </c>
-      <c r="F87">
-        <v>0.03855818108207108</v>
-      </c>
-      <c r="G87">
         <v>6.773626866508438</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:5">
       <c r="A88" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B88">
         <v>10</v>
@@ -2794,21 +2284,15 @@
         <v>187475</v>
       </c>
       <c r="D88">
-        <v>385.46</v>
+        <v>0.02594302910807866</v>
       </c>
       <c r="E88">
-        <v>49310</v>
-      </c>
-      <c r="F88">
-        <v>0.02594302910807866</v>
-      </c>
-      <c r="G88">
         <v>3.801967146623403</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:5">
       <c r="A89" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B89">
         <v>6</v>
@@ -2817,21 +2301,15 @@
         <v>417500</v>
       </c>
       <c r="D89">
-        <v>141.041</v>
+        <v>0.04254082146326246</v>
       </c>
       <c r="E89">
-        <v>50016</v>
-      </c>
-      <c r="F89">
-        <v>0.04254082146326246</v>
-      </c>
-      <c r="G89">
         <v>8.347328854766475</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:5">
       <c r="A90" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B90">
         <v>5</v>
@@ -2840,21 +2318,15 @@
         <v>229900</v>
       </c>
       <c r="D90">
-        <v>146.172</v>
+        <v>0.03420627753605342</v>
       </c>
       <c r="E90">
-        <v>44279</v>
-      </c>
-      <c r="F90">
-        <v>0.03420627753605342</v>
-      </c>
-      <c r="G90">
         <v>5.192077508525486</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:5">
       <c r="A91" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B91">
         <v>10</v>
@@ -2863,21 +2335,15 @@
         <v>98000</v>
       </c>
       <c r="D91">
-        <v>112.031</v>
+        <v>0.08926100811382563</v>
       </c>
       <c r="E91">
-        <v>45325</v>
-      </c>
-      <c r="F91">
-        <v>0.08926100811382563</v>
-      </c>
-      <c r="G91">
         <v>2.162162162162162</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:5">
       <c r="A92" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B92">
         <v>39</v>
@@ -2886,21 +2352,15 @@
         <v>179900</v>
       </c>
       <c r="D92">
-        <v>176.565</v>
+        <v>0.2208818282219013</v>
       </c>
       <c r="E92">
-        <v>46701</v>
-      </c>
-      <c r="F92">
-        <v>0.2208818282219013</v>
-      </c>
-      <c r="G92">
         <v>3.852165906511638</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:5">
       <c r="A93" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2909,21 +2369,15 @@
         <v>525000</v>
       </c>
       <c r="D93">
-        <v>134.3</v>
+        <v>0.007446016381236038</v>
       </c>
       <c r="E93">
-        <v>90608</v>
-      </c>
-      <c r="F93">
-        <v>0.007446016381236038</v>
-      </c>
-      <c r="G93">
         <v>5.794190358467244</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:5">
       <c r="A94" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B94">
         <v>15</v>
@@ -2932,21 +2386,15 @@
         <v>274900</v>
       </c>
       <c r="D94">
-        <v>396.415</v>
+        <v>0.03783913323158811</v>
       </c>
       <c r="E94">
-        <v>45152</v>
-      </c>
-      <c r="F94">
-        <v>0.03783913323158811</v>
-      </c>
-      <c r="G94">
         <v>6.088323883770376</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:5">
       <c r="A95" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -2955,21 +2403,15 @@
         <v>267450</v>
       </c>
       <c r="D95">
-        <v>160.869</v>
+        <v>0.02486495222821053</v>
       </c>
       <c r="E95">
-        <v>53610</v>
-      </c>
-      <c r="F95">
-        <v>0.02486495222821053</v>
-      </c>
-      <c r="G95">
         <v>4.988808058198098</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:5">
       <c r="A96" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B96">
         <v>63</v>
@@ -2978,21 +2420,15 @@
         <v>182500</v>
       </c>
       <c r="D96">
-        <v>121.348</v>
+        <v>0.5191680126578107</v>
       </c>
       <c r="E96">
-        <v>49859</v>
-      </c>
-      <c r="F96">
-        <v>0.5191680126578107</v>
-      </c>
-      <c r="G96">
         <v>3.660322108345535</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:5">
       <c r="A97" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B97">
         <v>2</v>
@@ -3001,9 +2437,9 @@
         <v>104950</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:5">
       <c r="A98" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B98">
         <v>233</v>
@@ -3012,21 +2448,15 @@
         <v>144900</v>
       </c>
       <c r="D98">
-        <v>396.466</v>
+        <v>0.5876922611270575</v>
       </c>
       <c r="E98">
-        <v>55784</v>
-      </c>
-      <c r="F98">
-        <v>0.5876922611270575</v>
-      </c>
-      <c r="G98">
         <v>2.597519001864334</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:5">
       <c r="A99" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B99">
         <v>45</v>
@@ -3035,21 +2465,15 @@
         <v>219900</v>
       </c>
       <c r="D99">
-        <v>2349.172</v>
+        <v>0.01915568549259058</v>
       </c>
       <c r="E99">
-        <v>65730</v>
-      </c>
-      <c r="F99">
-        <v>0.01915568549259058</v>
-      </c>
-      <c r="G99">
         <v>3.345504335919671</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:5">
       <c r="A100" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B100">
         <v>9</v>
@@ -3058,21 +2482,15 @@
         <v>324900</v>
       </c>
       <c r="D100">
-        <v>97.58499999999999</v>
+        <v>0.09222728903007635</v>
       </c>
       <c r="E100">
-        <v>45244</v>
-      </c>
-      <c r="F100">
-        <v>0.09222728903007635</v>
-      </c>
-      <c r="G100">
         <v>7.181062682344621</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:5">
       <c r="A101" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B101">
         <v>5</v>
@@ -3081,15 +2499,12 @@
         <v>575000</v>
       </c>
       <c r="D101">
-        <v>246.191</v>
-      </c>
-      <c r="F101">
         <v>0.02030943454472341</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:5">
       <c r="A102" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B102">
         <v>4</v>
@@ -3098,21 +2513,15 @@
         <v>295450</v>
       </c>
       <c r="D102">
-        <v>169.544</v>
+        <v>0.02359269570141084</v>
       </c>
       <c r="E102">
-        <v>46927</v>
-      </c>
-      <c r="F102">
-        <v>0.02359269570141084</v>
-      </c>
-      <c r="G102">
         <v>6.295949027212479</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:5">
       <c r="A103" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B103">
         <v>3</v>
@@ -3121,21 +2530,15 @@
         <v>149900</v>
       </c>
       <c r="D103">
-        <v>195.846</v>
+        <v>0.01531815814466468</v>
       </c>
       <c r="E103">
-        <v>56884</v>
-      </c>
-      <c r="F103">
-        <v>0.01531815814466468</v>
-      </c>
-      <c r="G103">
         <v>2.635187398917095</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:5">
       <c r="A104" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B104">
         <v>27</v>
@@ -3144,21 +2547,15 @@
         <v>369900</v>
       </c>
       <c r="D104">
-        <v>1484.338</v>
+        <v>0.01818992709207741</v>
       </c>
       <c r="E104">
-        <v>66428</v>
-      </c>
-      <c r="F104">
-        <v>0.01818992709207741</v>
-      </c>
-      <c r="G104">
         <v>5.568434997290299</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:5">
       <c r="A105" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B105">
         <v>19</v>
@@ -3167,21 +2564,15 @@
         <v>255000</v>
       </c>
       <c r="D105">
-        <v>430.449</v>
+        <v>0.04413995618528559</v>
       </c>
       <c r="E105">
-        <v>57970</v>
-      </c>
-      <c r="F105">
-        <v>0.04413995618528559</v>
-      </c>
-      <c r="G105">
         <v>4.39882697947214</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:5">
       <c r="A106" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B106">
         <v>3</v>
@@ -3190,21 +2581,15 @@
         <v>349000</v>
       </c>
       <c r="D106">
-        <v>180.93</v>
+        <v>0.0165809981760902</v>
       </c>
       <c r="E106">
-        <v>54972</v>
-      </c>
-      <c r="F106">
-        <v>0.0165809981760902</v>
-      </c>
-      <c r="G106">
         <v>6.348686604089354</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:5">
       <c r="A107" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B107">
         <v>10</v>
@@ -3213,21 +2598,15 @@
         <v>562500</v>
       </c>
       <c r="D107">
-        <v>500.915</v>
+        <v>0.01996346685565415</v>
       </c>
       <c r="E107">
-        <v>71489</v>
-      </c>
-      <c r="F107">
-        <v>0.01996346685565415</v>
-      </c>
-      <c r="G107">
         <v>7.868343381499252</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:5">
       <c r="A108" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B108">
         <v>38</v>
@@ -3236,21 +2615,15 @@
         <v>327403</v>
       </c>
       <c r="D108">
-        <v>1339.182</v>
+        <v>0.02837553073443341</v>
       </c>
       <c r="E108">
-        <v>65834</v>
-      </c>
-      <c r="F108">
-        <v>0.02837553073443341</v>
-      </c>
-      <c r="G108">
         <v>4.973159765470729</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:5">
       <c r="A109" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B109">
         <v>18</v>
@@ -3259,21 +2632,15 @@
         <v>265975</v>
       </c>
       <c r="D109">
-        <v>314.34</v>
+        <v>0.05726283641916396</v>
       </c>
       <c r="E109">
-        <v>53939</v>
-      </c>
-      <c r="F109">
-        <v>0.05726283641916396</v>
-      </c>
-      <c r="G109">
         <v>4.931033204175087</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:5">
       <c r="A110" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B110">
         <v>16</v>
@@ -3282,21 +2649,15 @@
         <v>264900</v>
       </c>
       <c r="D110">
-        <v>228.073</v>
+        <v>0.07015297733620375</v>
       </c>
       <c r="E110">
-        <v>63052</v>
-      </c>
-      <c r="F110">
-        <v>0.07015297733620375</v>
-      </c>
-      <c r="G110">
         <v>4.201294169891518</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:5">
       <c r="A111" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B111">
         <v>3</v>
@@ -3305,21 +2666,15 @@
         <v>195000</v>
       </c>
       <c r="D111">
-        <v>1081.152</v>
+        <v>0.00277481797194104</v>
       </c>
       <c r="E111">
-        <v>58500</v>
-      </c>
-      <c r="F111">
-        <v>0.00277481797194104</v>
-      </c>
-      <c r="G111">
         <v>3.333333333333333</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:5">
       <c r="A112" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B112">
         <v>35</v>
@@ -3328,21 +2683,15 @@
         <v>160000</v>
       </c>
       <c r="D112">
-        <v>335.342</v>
+        <v>0.1043710599924853</v>
       </c>
       <c r="E112">
-        <v>51140</v>
-      </c>
-      <c r="F112">
-        <v>0.1043710599924853</v>
-      </c>
-      <c r="G112">
         <v>3.128666405944466</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:5">
       <c r="A113" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B113">
         <v>8</v>
@@ -3351,21 +2700,15 @@
         <v>245000</v>
       </c>
       <c r="D113">
-        <v>99.443</v>
+        <v>0.08044809589413031</v>
       </c>
       <c r="E113">
-        <v>44803</v>
-      </c>
-      <c r="F113">
-        <v>0.08044809589413031</v>
-      </c>
-      <c r="G113">
         <v>5.468383813583912</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:5">
       <c r="A114" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B114">
         <v>8</v>
@@ -3374,21 +2717,15 @@
         <v>154450</v>
       </c>
       <c r="D114">
-        <v>188.33</v>
+        <v>0.04247862794031752</v>
       </c>
       <c r="E114">
-        <v>49274</v>
-      </c>
-      <c r="F114">
-        <v>0.04247862794031752</v>
-      </c>
-      <c r="G114">
         <v>3.134513130657142</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:5">
       <c r="A115" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B115">
         <v>24</v>
@@ -3397,21 +2734,15 @@
         <v>432400</v>
       </c>
       <c r="D115">
-        <v>436.317</v>
+        <v>0.05500587875329176</v>
       </c>
       <c r="E115">
-        <v>52971</v>
-      </c>
-      <c r="F115">
-        <v>0.05500587875329176</v>
-      </c>
-      <c r="G115">
         <v>8.162957089728343</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:5">
       <c r="A116" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -3420,21 +2751,15 @@
         <v>945000</v>
       </c>
       <c r="D116">
-        <v>432.858</v>
+        <v>0.002310226448396472</v>
       </c>
       <c r="E116">
-        <v>63449</v>
-      </c>
-      <c r="F116">
-        <v>0.002310226448396472</v>
-      </c>
-      <c r="G116">
         <v>14.8938517549528</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:5">
       <c r="A117" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B117">
         <v>2</v>
@@ -3443,9 +2768,9 @@
         <v>165000</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:5">
       <c r="A118" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B118">
         <v>27</v>
@@ -3454,21 +2779,15 @@
         <v>299999</v>
       </c>
       <c r="D118">
-        <v>418.373</v>
+        <v>0.06453571334670259</v>
       </c>
       <c r="E118">
-        <v>53570</v>
-      </c>
-      <c r="F118">
-        <v>0.06453571334670259</v>
-      </c>
-      <c r="G118">
         <v>5.600130670151204</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:5">
       <c r="A119" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B119">
         <v>3</v>
@@ -3477,21 +2796,15 @@
         <v>249900</v>
       </c>
       <c r="D119">
-        <v>117.841</v>
+        <v>0.02545803243353332</v>
       </c>
       <c r="E119">
-        <v>58425</v>
-      </c>
-      <c r="F119">
-        <v>0.02545803243353332</v>
-      </c>
-      <c r="G119">
         <v>4.277278562259307</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:5">
       <c r="A120" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B120">
         <v>30</v>
@@ -3500,21 +2813,15 @@
         <v>233892</v>
       </c>
       <c r="D120">
-        <v>345.831</v>
+        <v>0.0867475732366387</v>
       </c>
       <c r="E120">
-        <v>50596</v>
-      </c>
-      <c r="F120">
-        <v>0.0867475732366387</v>
-      </c>
-      <c r="G120">
         <v>4.622736975254961</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:5">
       <c r="A121" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B121">
         <v>24</v>
@@ -3523,21 +2830,15 @@
         <v>144950</v>
       </c>
       <c r="D121">
-        <v>206.655</v>
+        <v>0.1161355882993395</v>
       </c>
       <c r="E121">
-        <v>57126</v>
-      </c>
-      <c r="F121">
-        <v>0.1161355882993395</v>
-      </c>
-      <c r="G121">
         <v>2.537373525189931</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:5">
       <c r="A122" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B122">
         <v>28</v>
@@ -3546,21 +2847,15 @@
         <v>234900</v>
       </c>
       <c r="D122">
-        <v>487.061</v>
+        <v>0.05748766581598609</v>
       </c>
       <c r="E122">
-        <v>48664</v>
-      </c>
-      <c r="F122">
-        <v>0.05748766581598609</v>
-      </c>
-      <c r="G122">
         <v>4.826976820647706</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:5">
       <c r="A123" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B123">
         <v>8</v>
@@ -3569,21 +2864,15 @@
         <v>161400</v>
       </c>
       <c r="D123">
-        <v>134.831</v>
+        <v>0.0593335360562482</v>
       </c>
       <c r="E123">
-        <v>47929</v>
-      </c>
-      <c r="F123">
-        <v>0.0593335360562482</v>
-      </c>
-      <c r="G123">
         <v>3.367481065743078</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:5">
       <c r="A124" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B124">
         <v>8</v>
@@ -3592,21 +2881,15 @@
         <v>117450</v>
       </c>
       <c r="D124">
-        <v>134.925</v>
+        <v>0.05929219937002038</v>
       </c>
       <c r="E124">
-        <v>46550</v>
-      </c>
-      <c r="F124">
-        <v>0.05929219937002038</v>
-      </c>
-      <c r="G124">
         <v>2.523093447905478</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:5">
       <c r="A125" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -3615,21 +2898,15 @@
         <v>127500</v>
       </c>
       <c r="D125">
-        <v>653.633</v>
+        <v>0.001529910515533946</v>
       </c>
       <c r="E125">
-        <v>58137</v>
-      </c>
-      <c r="F125">
-        <v>0.001529910515533946</v>
-      </c>
-      <c r="G125">
         <v>2.193095618968987</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:5">
       <c r="A126" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B126">
         <v>37</v>
@@ -3638,21 +2915,15 @@
         <v>323000</v>
       </c>
       <c r="D126">
-        <v>390.992</v>
+        <v>0.09463109219625977</v>
       </c>
       <c r="E126">
-        <v>52279</v>
-      </c>
-      <c r="F126">
-        <v>0.09463109219625977</v>
-      </c>
-      <c r="G126">
         <v>6.178389028099237</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:5">
       <c r="A127" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B127">
         <v>11</v>
@@ -3661,21 +2932,15 @@
         <v>145000</v>
       </c>
       <c r="D127">
-        <v>640.384</v>
+        <v>0.01717719368378973</v>
       </c>
       <c r="E127">
-        <v>54423</v>
-      </c>
-      <c r="F127">
-        <v>0.01717719368378973</v>
-      </c>
-      <c r="G127">
         <v>2.664314719879463</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:5">
       <c r="A128" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B128">
         <v>24</v>
@@ -3684,21 +2949,15 @@
         <v>167000</v>
       </c>
       <c r="D128">
-        <v>231.783</v>
+        <v>0.1035451262603383</v>
       </c>
       <c r="E128">
-        <v>53655</v>
-      </c>
-      <c r="F128">
-        <v>0.1035451262603383</v>
-      </c>
-      <c r="G128">
         <v>3.112477867859472</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:5">
       <c r="A129" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B129">
         <v>6</v>
@@ -3707,21 +2966,15 @@
         <v>290000</v>
       </c>
       <c r="D129">
-        <v>380.688</v>
+        <v>0.01576093809103518</v>
       </c>
       <c r="E129">
-        <v>77911</v>
-      </c>
-      <c r="F129">
-        <v>0.01576093809103518</v>
-      </c>
-      <c r="G129">
         <v>3.722195838841755</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:5">
       <c r="A130" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B130">
         <v>52</v>
@@ -3730,21 +2983,15 @@
         <v>345000</v>
       </c>
       <c r="D130">
-        <v>1057.597</v>
+        <v>0.04916806685344229</v>
       </c>
       <c r="E130">
-        <v>52942</v>
-      </c>
-      <c r="F130">
-        <v>0.04916806685344229</v>
-      </c>
-      <c r="G130">
         <v>6.516565297873144</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:5">
       <c r="A131" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B131">
         <v>25</v>
@@ -3753,21 +3000,15 @@
         <v>190000</v>
       </c>
       <c r="D131">
-        <v>1034.123</v>
+        <v>0.02417507395155122</v>
       </c>
       <c r="E131">
-        <v>59941</v>
-      </c>
-      <c r="F131">
-        <v>0.02417507395155122</v>
-      </c>
-      <c r="G131">
         <v>3.169783620560218</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:5">
       <c r="A132" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B132">
         <v>8</v>
@@ -3776,21 +3017,15 @@
         <v>282450</v>
       </c>
       <c r="D132">
-        <v>277.494</v>
+        <v>0.02882945216833517</v>
       </c>
       <c r="E132">
-        <v>43362</v>
-      </c>
-      <c r="F132">
-        <v>0.02882945216833517</v>
-      </c>
-      <c r="G132">
         <v>6.513767815137678</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:5">
       <c r="A133" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B133">
         <v>4</v>
@@ -3799,21 +3034,15 @@
         <v>384950</v>
       </c>
       <c r="D133">
-        <v>241.922</v>
+        <v>0.01653425484246989</v>
       </c>
       <c r="E133">
-        <v>60284</v>
-      </c>
-      <c r="F133">
-        <v>0.01653425484246989</v>
-      </c>
-      <c r="G133">
         <v>6.385608121557959</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:5">
       <c r="A134" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -3822,21 +3051,15 @@
         <v>219900</v>
       </c>
       <c r="D134">
-        <v>98.196</v>
+        <v>0.01018371420424457</v>
       </c>
       <c r="E134">
-        <v>58294</v>
-      </c>
-      <c r="F134">
-        <v>0.01018371420424457</v>
-      </c>
-      <c r="G134">
         <v>3.772257865303462</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:5">
       <c r="A135" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B135">
         <v>7</v>
@@ -3845,21 +3068,15 @@
         <v>260000</v>
       </c>
       <c r="D135">
-        <v>283.885</v>
+        <v>0.02465787202564419</v>
       </c>
       <c r="E135">
-        <v>49151</v>
-      </c>
-      <c r="F135">
-        <v>0.02465787202564419</v>
-      </c>
-      <c r="G135">
         <v>5.289821163353746</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:5">
       <c r="A136" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B136">
         <v>3</v>
@@ -3868,21 +3085,15 @@
         <v>129900</v>
       </c>
       <c r="D136">
-        <v>166.334</v>
+        <v>0.018035999855712</v>
       </c>
       <c r="E136">
-        <v>56947</v>
-      </c>
-      <c r="F136">
-        <v>0.018035999855712</v>
-      </c>
-      <c r="G136">
         <v>2.281068361810104</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:5">
       <c r="A137" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -3891,21 +3102,15 @@
         <v>340000</v>
       </c>
       <c r="D137">
-        <v>124.118</v>
+        <v>0.00805684912744324</v>
       </c>
       <c r="E137">
-        <v>58009</v>
-      </c>
-      <c r="F137">
-        <v>0.00805684912744324</v>
-      </c>
-      <c r="G137">
         <v>5.86115947525384</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:5">
       <c r="A138" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B138">
         <v>48</v>
@@ -3914,21 +3119,15 @@
         <v>207450</v>
       </c>
       <c r="D138">
-        <v>650.039</v>
+        <v>0.07384172334275328</v>
       </c>
       <c r="E138">
-        <v>56343</v>
-      </c>
-      <c r="F138">
-        <v>0.07384172334275328</v>
-      </c>
-      <c r="G138">
         <v>3.68191257121559</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:5">
       <c r="A139" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -3937,21 +3136,15 @@
         <v>228900</v>
       </c>
       <c r="D139">
-        <v>113.104</v>
+        <v>0.008841420285754704</v>
       </c>
       <c r="E139">
-        <v>50464</v>
-      </c>
-      <c r="F139">
-        <v>0.008841420285754704</v>
-      </c>
-      <c r="G139">
         <v>4.535906785034876</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:5">
       <c r="A140" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B140">
         <v>12</v>
@@ -3960,21 +3153,15 @@
         <v>400100</v>
       </c>
       <c r="D140">
-        <v>300.658</v>
+        <v>0.03991245867397508</v>
       </c>
       <c r="E140">
-        <v>55750</v>
-      </c>
-      <c r="F140">
-        <v>0.03991245867397508</v>
-      </c>
-      <c r="G140">
         <v>7.176681614349776</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:5">
       <c r="A141" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B141">
         <v>2</v>
@@ -3983,21 +3170,15 @@
         <v>330000</v>
       </c>
       <c r="D141">
-        <v>257.001</v>
+        <v>0.007782070886883709</v>
       </c>
       <c r="E141">
-        <v>50872</v>
-      </c>
-      <c r="F141">
-        <v>0.007782070886883709</v>
-      </c>
-      <c r="G141">
         <v>6.486869004560465</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:5">
       <c r="A142" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B142">
         <v>8</v>
@@ -4006,15 +3187,9 @@
         <v>242250</v>
       </c>
       <c r="D142">
-        <v>207.842</v>
+        <v>0.0384907766476458</v>
       </c>
       <c r="E142">
-        <v>44299</v>
-      </c>
-      <c r="F142">
-        <v>0.0384907766476458</v>
-      </c>
-      <c r="G142">
         <v>5.46852073410235</v>
       </c>
     </row>

</xml_diff>